<commit_message>
new version of db
</commit_message>
<xml_diff>
--- a/fontes_db/fornecedores_pref/Eleições 2012 - Despesas Comitê Coligação Prefeito e Vice-Prefeito.xlsx
+++ b/fontes_db/fornecedores_pref/Eleições 2012 - Despesas Comitê Coligação Prefeito e Vice-Prefeito.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renatoaranha/PycharmProjects/portaltransparenciamacae/fontes_db/fornecedores_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renatoaranha/PycharmProjects/portaltransparenciamacae/fontes_db/fornec_pref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E97537-21EF-EB41-A56F-8D16885F3440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA6ABD6-3596-AE4A-848C-E0ED75990E90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{427EC1EA-39E8-46FC-A777-C6ED2A2EB76D}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="123">
   <si>
     <t>Cód. Eleição</t>
   </si>
@@ -416,6 +416,9 @@
   </si>
   <si>
     <t>CNPJ</t>
+  </si>
+  <si>
+    <t>DESPESAS BANCÁRIAS</t>
   </si>
 </sst>
 </file>
@@ -1451,7 +1454,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9ADD391F-3851-4959-BE2C-B6E6BAB17387}" name="Tabela dinâmica11" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9ADD391F-3851-4959-BE2C-B6E6BAB17387}" name="Tabela dinâmica11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A1:D14" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="22">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -4173,10 +4176,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F436C8-38DF-4CFC-ADAF-9D62293D3061}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4328,6 +4331,17 @@
         <v>1.2463626284877032E-2</v>
       </c>
     </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13">
+        <v>3.1330840048811076E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -4338,7 +4352,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>